<commit_message>
corrected the wasm prefix at a3 task
</commit_message>
<xml_diff>
--- a/mahofmahof/evidence.xlsx
+++ b/mahofmahof/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="20"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="88">
   <si>
     <t>TxHash</t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>3841FF81EAA9EAA672AE16FAC9E43AD5BED81D8E42B91788FC7C6A01D8C2319E</t>
-  </si>
-  <si>
-    <t>wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-89/gonballs</t>
   </si>
   <si>
     <t>france</t>
@@ -800,10 +797,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -838,10 +835,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -876,10 +873,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -914,10 +911,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -960,34 +957,34 @@
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
         <v>51</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
         <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
         <v>55</v>
-      </c>
-      <c r="B5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1023,23 +1020,23 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
         <v>30</v>
@@ -1047,10 +1044,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1086,34 +1083,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1148,34 +1145,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1210,34 +1207,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1272,15 +1269,15 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>30</v>
@@ -1288,15 +1285,15 @@
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>30</v>
@@ -1371,50 +1368,50 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1429,7 +1426,7 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1449,31 +1446,31 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
@@ -1481,18 +1478,18 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1677,13 +1674,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
         <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1698,7 +1695,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1728,13 +1725,13 @@
         <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1806,7 +1803,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1827,16 +1825,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1924,10 +1922,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1962,11 +1960,11 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>42</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
STAGE 3 B1-B2 upload
</commit_message>
<xml_diff>
--- a/mahofmahof/evidence.xlsx
+++ b/mahofmahof/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="92">
   <si>
     <t>TxHash</t>
   </si>
@@ -302,6 +302,18 @@
   </si>
   <si>
     <t>F088C9A39FA9CE0E24290B2958C68A77DB44C8CE466E3F6C260366366494740B</t>
+  </si>
+  <si>
+    <t>63C72C2B34FF907482997050C7C87A1E65A2308C5C895B1D9DF9470A3674EDD0</t>
+  </si>
+  <si>
+    <t>B3AE31C334892AAD882BE02E2DFBDE82F685EFC4425404D0A0F6350BD921D24A</t>
+  </si>
+  <si>
+    <t>734218E2AC1A0F7E91FC306BF729ECEC36CC69819E18D12E81EA1D7F5CAD3FC5</t>
+  </si>
+  <si>
+    <t>EA31E12D2B39908F31FD3CEE8C18951D6D2C1BD221D3493DA861AD7E7975EFDA</t>
   </si>
 </sst>
 </file>
@@ -1504,6 +1516,78 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="85" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="82.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1531,7 +1615,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -1565,74 +1649,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
@@ -1695,7 +1711,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update  A13 4 tx hash there was a typo
there was a typo it should be 11BABDAB50AA79B8E9131232AD6F50714B21482DA957EB5F9B6C10FE14DC07CE but it was 1BABDAB50AA79B8E9131232AD6F50714B21482DA957EB5F9B6C10FE14DC07CE i have corrected that typo
</commit_message>
<xml_diff>
--- a/mahofmahof/evidence.xlsx
+++ b/mahofmahof/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="22"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -208,9 +208,6 @@
     <t>uptick_7000-2</t>
   </si>
   <si>
-    <t>1BABDAB50AA79B8E9131232AD6F50714B21482DA957EB5F9B6C10FE14DC07CE</t>
-  </si>
-  <si>
     <t>2E53A0E808F080E5D39F35E6F3D3147F34A20022568A9DC10235E36B8BABB5A2</t>
   </si>
   <si>
@@ -314,6 +311,9 @@
   </si>
   <si>
     <t>EA31E12D2B39908F31FD3CEE8C18951D6D2C1BD221D3493DA861AD7E7975EFDA</t>
+  </si>
+  <si>
+    <t>11BABDAB50AA79B8E9131232AD6F50714B21482DA957EB5F9B6C10FE14DC07CE</t>
   </si>
 </sst>
 </file>
@@ -941,8 +941,8 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,7 +993,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
         <v>53</v>
@@ -1032,7 +1032,7 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>51</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>55</v>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
         <v>30</v>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
         <v>55</v>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>51</v>
@@ -1103,7 +1103,7 @@
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -1111,7 +1111,7 @@
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
         <v>55</v>
@@ -1119,7 +1119,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>51</v>
@@ -1165,7 +1165,7 @@
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -1173,7 +1173,7 @@
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
         <v>53</v>
@@ -1181,7 +1181,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>51</v>
@@ -1227,7 +1227,7 @@
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
         <v>53</v>
@@ -1235,7 +1235,7 @@
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -1243,7 +1243,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
         <v>53</v>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>51</v>
@@ -1289,7 +1289,7 @@
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>30</v>
@@ -1297,7 +1297,7 @@
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
         <v>55</v>
@@ -1305,7 +1305,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>30</v>
@@ -1380,7 +1380,7 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>51</v>
@@ -1388,7 +1388,7 @@
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
         <v>53</v>
@@ -1396,7 +1396,7 @@
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
         <v>55</v>
@@ -1412,7 +1412,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
         <v>34</v>
@@ -1420,7 +1420,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
         <v>53</v>
@@ -1458,7 +1458,7 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>51</v>
@@ -1466,7 +1466,7 @@
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
         <v>55</v>
@@ -1474,7 +1474,7 @@
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
         <v>53</v>
@@ -1482,7 +1482,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
@@ -1490,7 +1490,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
         <v>53</v>
@@ -1498,7 +1498,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
         <v>55</v>
@@ -1532,12 +1532,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1552,7 +1552,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -1568,12 +1568,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected the 4th txhash at A20
it was a copy paste mistake corrected now
</commit_message>
<xml_diff>
--- a/mahofmahof/evidence.xlsx
+++ b/mahofmahof/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="13"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="93">
   <si>
     <t>TxHash</t>
   </si>
@@ -314,6 +314,9 @@
   </si>
   <si>
     <t>11BABDAB50AA79B8E9131232AD6F50714B21482DA957EB5F9B6C10FE14DC07CE</t>
+  </si>
+  <si>
+    <t>C1D961ECB37C47BA7500D399EC9AD5E99D38D72B6A0047BD190F33DF83977485</t>
   </si>
 </sst>
 </file>
@@ -941,7 +944,7 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1438,8 +1441,8 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,7 +1485,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>

</xml_diff>